<commit_message>
Lab 2 - Question 6 Done
</commit_message>
<xml_diff>
--- a/Lab2/TimeComplexity.xlsx
+++ b/Lab2/TimeComplexity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/805fd1da7aba8867/Documents/Universitet/HT-2021/Algoritmer och Datastrukturer/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\OneDrive\Documents\Universitet\HT-2021\Algoritmer och Datastrukturer\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="637" documentId="8_{17440A54-2BD4-42CB-828B-E38889D6206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1482432-0EB3-4144-ADA1-28B08ED4FF8F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0649A155-F993-45A6-BF78-055D664C7B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E899B47F-0D67-46C6-83CC-3E08B70027EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E899B47F-0D67-46C6-83CC-3E08B70027EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Quick Sort</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Exercise 5</t>
+  </si>
+  <si>
+    <t>Exercise 6</t>
+  </si>
+  <si>
+    <t>Quick Sort First Partitioning</t>
+  </si>
+  <si>
+    <t>Quick Sort Median Of Three</t>
   </si>
 </sst>
 </file>
@@ -231,7 +240,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -709,7 +718,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1034,7 +1042,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1485,7 +1493,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1936,7 +1944,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2387,7 +2395,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2808,7 +2816,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3114,10 +3121,1129 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort First Partitioning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AI$5:$AI$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$5:$AJ$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.0999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4299999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1359999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4279999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2443999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30603900000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92679</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6861699999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.01539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.117709999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79.238900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502.21546599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-73EA-4C6B-926D-7CFDECA306D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AK$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort Median Of Three</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AI$5:$AI$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.68E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4299999999999994E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2499999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.53E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.322579</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99053999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6443699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2691099999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.404440000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>81.338099999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502.21546599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73EA-4C6B-926D-7CFDECA306D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="16186111"/>
+        <c:axId val="16184447"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="16186111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16184447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="16184447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16186111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort First Partitioning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AI$5:$AI$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$5:$AJ$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.0999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4299999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1359999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4279999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2443999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30603900000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92679</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6861699999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.01539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.117709999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79.238900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502.21546599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-372E-4427-A60C-B329205D2F9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AK$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort Median Of Three</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AI$5:$AI$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.68E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4299999999999994E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2499999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.53E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.322579</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99053999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6443699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2691099999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.404440000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>81.338099999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502.21546599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-372E-4427-A60C-B329205D2F9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="16186111"/>
+        <c:axId val="16184447"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="16186111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16184447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="16184447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7.4280000000000023E-3"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16186111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3593,7 +4719,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4066,7 +5192,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4542,7 +5668,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4887,7 +6013,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5211,7 +6336,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6015,7 +7140,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6466,7 +7591,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6917,7 +8042,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7565,6 +8690,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10465,6 +11670,1046 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -15071,16 +17316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>676965</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>258795</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>147055</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>483664</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>355890</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>32756</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15107,11 +17352,85 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>465194</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>470296</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138453</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0493FF9-D356-4FFE-9A97-3F4F6593C813}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>450736</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>17009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>140834</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28A35CE4-A292-44D4-9C31-2B5FDFBB1010}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -15407,10 +17726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B459674-4D5A-4045-ABAA-D30208F2DC5A}">
-  <dimension ref="B1:AK35"/>
+  <dimension ref="B1:AL35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF41" sqref="AF41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15419,11 +17738,11 @@
     <col min="2" max="2" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2"/>
     <col min="8" max="8" width="17.42578125" style="2" customWidth="1"/>
     <col min="9" max="10" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="2"/>
     <col min="14" max="14" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -15436,29 +17755,33 @@
     <col min="21" max="21" width="9.140625" style="2"/>
     <col min="22" max="22" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="2"/>
-    <col min="25" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.140625" style="2"/>
-    <col min="31" max="31" width="10.42578125" style="2" customWidth="1"/>
-    <col min="32" max="34" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="2"/>
+    <col min="30" max="30" width="18.42578125" style="2" customWidth="1"/>
+    <col min="31" max="32" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="2"/>
+    <col min="36" max="37" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" ht="61.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:38" ht="61.5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="2:37" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:38" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -15471,8 +17794,14 @@
       <c r="V3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AD3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -15542,15 +17871,30 @@
       <c r="AB4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
+      <c r="AD4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL4" s="10"/>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -15629,8 +17973,32 @@
         <f t="shared" si="0"/>
         <v>122.2092</v>
       </c>
+      <c r="AD5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>61</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>73</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>10000000</v>
+      </c>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AJ5" s="2">
+        <f>AE5*10^-6</f>
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="AK5" s="2">
+        <f>AF5*10^-6</f>
+        <v>7.2999999999999999E-5</v>
+      </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>50</v>
       </c>
@@ -15709,8 +18077,32 @@
         <f t="shared" ref="AB6:AB35" si="9">T6*10^-6</f>
         <v>69.877099999999999</v>
       </c>
+      <c r="AD6" s="2">
+        <v>50</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>443</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>368</v>
+      </c>
+      <c r="AG6" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="2">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="2">
+        <f>AE6*10^-6</f>
+        <v>4.4299999999999998E-4</v>
+      </c>
+      <c r="AK6" s="2">
+        <f>AF6*10^-6</f>
+        <v>3.68E-4</v>
+      </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>100</v>
       </c>
@@ -15789,8 +18181,32 @@
         <f t="shared" si="9"/>
         <v>58.879799999999996</v>
       </c>
+      <c r="AD7" s="2">
+        <v>100</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>1136</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>943</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>100000</v>
+      </c>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="2">
+        <v>100</v>
+      </c>
+      <c r="AJ7" s="2">
+        <f>AE7*10^-6</f>
+        <v>1.1359999999999999E-3</v>
+      </c>
+      <c r="AK7" s="2">
+        <f>AF7*10^-6</f>
+        <v>9.4299999999999994E-4</v>
+      </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>500</v>
       </c>
@@ -15869,8 +18285,32 @@
         <f t="shared" si="9"/>
         <v>44.283799999999999</v>
       </c>
+      <c r="AD8" s="2">
+        <v>500</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>7428</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>6250</v>
+      </c>
+      <c r="AG8" s="7">
+        <v>100000</v>
+      </c>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="2">
+        <v>500</v>
+      </c>
+      <c r="AJ8" s="2">
+        <f>AE8*10^-6</f>
+        <v>7.4279999999999997E-3</v>
+      </c>
+      <c r="AK8" s="2">
+        <f>AF8*10^-6</f>
+        <v>6.2499999999999995E-3</v>
+      </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1000</v>
       </c>
@@ -15949,8 +18389,32 @@
         <f t="shared" si="9"/>
         <v>34.860199999999999</v>
       </c>
+      <c r="AD9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>22444</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>25300</v>
+      </c>
+      <c r="AG9" s="7">
+        <v>100000</v>
+      </c>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f>AE9*10^-6</f>
+        <v>2.2443999999999999E-2</v>
+      </c>
+      <c r="AK9" s="2">
+        <f>AF9*10^-6</f>
+        <v>2.53E-2</v>
+      </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>5000</v>
       </c>
@@ -16029,8 +18493,32 @@
         <f t="shared" si="9"/>
         <v>33.987699999999997</v>
       </c>
+      <c r="AD10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>306039</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>322579</v>
+      </c>
+      <c r="AG10" s="7">
+        <v>1000</v>
+      </c>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f>AE10*10^-6</f>
+        <v>0.30603900000000001</v>
+      </c>
+      <c r="AK10" s="2">
+        <f>AF10*10^-6</f>
+        <v>0.322579</v>
+      </c>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>10000</v>
       </c>
@@ -16109,8 +18597,32 @@
         <f t="shared" si="9"/>
         <v>33.3643</v>
       </c>
+      <c r="AD11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>926790</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>990540</v>
+      </c>
+      <c r="AG11" s="7">
+        <v>100</v>
+      </c>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f>AE11*10^-6</f>
+        <v>0.92679</v>
+      </c>
+      <c r="AK11" s="2">
+        <f>AF11*10^-6</f>
+        <v>0.99053999999999998</v>
+      </c>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>50000</v>
       </c>
@@ -16189,8 +18701,32 @@
         <f t="shared" si="9"/>
         <v>32.376100000000001</v>
       </c>
+      <c r="AD12" s="2">
+        <v>50000</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>3686170</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>3644370</v>
+      </c>
+      <c r="AG12" s="7">
+        <v>100</v>
+      </c>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="2">
+        <v>50000</v>
+      </c>
+      <c r="AJ12" s="2">
+        <f>AE12*10^-6</f>
+        <v>3.6861699999999997</v>
+      </c>
+      <c r="AK12" s="2">
+        <f>AF12*10^-6</f>
+        <v>3.6443699999999999</v>
+      </c>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>100000</v>
       </c>
@@ -16269,8 +18805,32 @@
         <f t="shared" si="9"/>
         <v>30.0764</v>
       </c>
+      <c r="AD13" s="2">
+        <v>100000</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>8015390</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>7269110</v>
+      </c>
+      <c r="AG13" s="7">
+        <v>10</v>
+      </c>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="2">
+        <v>100000</v>
+      </c>
+      <c r="AJ13" s="2">
+        <f>AE13*10^-6</f>
+        <v>8.01539</v>
+      </c>
+      <c r="AK13" s="2">
+        <f>AF13*10^-6</f>
+        <v>7.2691099999999995</v>
+      </c>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>500000</v>
       </c>
@@ -16349,8 +18909,32 @@
         <f t="shared" si="9"/>
         <v>29.2393</v>
       </c>
+      <c r="AD14" s="2">
+        <v>500000</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>40117710</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>38404440</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>10</v>
+      </c>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="2">
+        <v>500000</v>
+      </c>
+      <c r="AJ14" s="2">
+        <f>AE14*10^-6</f>
+        <v>40.117709999999995</v>
+      </c>
+      <c r="AK14" s="2">
+        <f>AF14*10^-6</f>
+        <v>38.404440000000001</v>
+      </c>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>1000000</v>
       </c>
@@ -16429,8 +19013,32 @@
         <f t="shared" si="9"/>
         <v>29.323699999999999</v>
       </c>
+      <c r="AD15" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>79238900</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>81338100</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="AJ15" s="2">
+        <f>AE15*10^-6</f>
+        <v>79.238900000000001</v>
+      </c>
+      <c r="AK15" s="2">
+        <f>AF15*10^-6</f>
+        <v>81.338099999999997</v>
+      </c>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>5000000</v>
       </c>
@@ -16504,6 +19112,30 @@
       <c r="AB16" s="2">
         <f t="shared" si="9"/>
         <v>30.005099999999999</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>476677033</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>502215466</v>
+      </c>
+      <c r="AG16" s="7">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="AJ16" s="2">
+        <f>AF16*10^-6</f>
+        <v>502.21546599999999</v>
+      </c>
+      <c r="AK16" s="2">
+        <f>AF16*10^-6</f>
+        <v>502.21546599999999</v>
       </c>
     </row>
     <row r="17" spans="14:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lab 2 - Question 7 Done
</commit_message>
<xml_diff>
--- a/Lab2/TimeComplexity.xlsx
+++ b/Lab2/TimeComplexity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\OneDrive\Documents\Universitet\HT-2021\Algoritmer och Datastrukturer\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0649A155-F993-45A6-BF78-055D664C7B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AAF5F-2596-4876-9FFD-7B5273C85C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E899B47F-0D67-46C6-83CC-3E08B70027EA}"/>
   </bookViews>
@@ -17728,8 +17728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B459674-4D5A-4045-ABAA-D30208F2DC5A}">
   <dimension ref="B1:AL35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF41" sqref="AF41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="74" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17990,11 +17990,11 @@
         <v>10</v>
       </c>
       <c r="AJ5" s="2">
-        <f>AE5*10^-6</f>
+        <f t="shared" ref="AJ5:AJ15" si="1">AE5*10^-6</f>
         <v>6.0999999999999999E-5</v>
       </c>
       <c r="AK5" s="2">
-        <f>AF5*10^-6</f>
+        <f t="shared" ref="AK5:AK15" si="2">AF5*10^-6</f>
         <v>7.2999999999999999E-5</v>
       </c>
     </row>
@@ -18018,15 +18018,15 @@
         <v>50</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I6:I16" si="1">C6*10^-6</f>
+        <f t="shared" ref="I6:I16" si="3">C6*10^-6</f>
         <v>2.61E-4</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J16" si="2">D6*10^-6</f>
+        <f t="shared" ref="J6:J16" si="4">D6*10^-6</f>
         <v>1.0889999999999999E-3</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K14" si="3">E6*10^-6</f>
+        <f t="shared" ref="K6:K14" si="5">E6*10^-6</f>
         <v>2.0999999999999998E-4</v>
       </c>
       <c r="N6" s="2">
@@ -18054,27 +18054,27 @@
         <v>1</v>
       </c>
       <c r="W6" s="2">
-        <f t="shared" ref="W6:W35" si="4">O6*10^-6</f>
+        <f t="shared" ref="W6:W35" si="6">O6*10^-6</f>
         <v>1.85E-4</v>
       </c>
       <c r="X6" s="2">
-        <f t="shared" ref="X6:X35" si="5">P6*10^-6</f>
+        <f t="shared" ref="X6:X35" si="7">P6*10^-6</f>
         <v>3.5279999999999999E-3</v>
       </c>
       <c r="Y6" s="2">
-        <f t="shared" ref="Y6:Y35" si="6">Q6*10^-6</f>
+        <f t="shared" ref="Y6:Y35" si="8">Q6*10^-6</f>
         <v>4.6313E-2</v>
       </c>
       <c r="Z6" s="2">
-        <f t="shared" ref="Z6:Z35" si="7">R6*10^-6</f>
+        <f t="shared" ref="Z6:Z35" si="9">R6*10^-6</f>
         <v>0.52966000000000002</v>
       </c>
       <c r="AA6" s="2">
-        <f t="shared" ref="AA6:AA35" si="8">S6*10^-6</f>
+        <f t="shared" ref="AA6:AA35" si="10">S6*10^-6</f>
         <v>6.8739999999999997</v>
       </c>
       <c r="AB6" s="2">
-        <f t="shared" ref="AB6:AB35" si="9">T6*10^-6</f>
+        <f t="shared" ref="AB6:AB35" si="11">T6*10^-6</f>
         <v>69.877099999999999</v>
       </c>
       <c r="AD6" s="2">
@@ -18094,11 +18094,11 @@
         <v>50</v>
       </c>
       <c r="AJ6" s="2">
-        <f>AE6*10^-6</f>
+        <f t="shared" si="1"/>
         <v>4.4299999999999998E-4</v>
       </c>
       <c r="AK6" s="2">
-        <f>AF6*10^-6</f>
+        <f t="shared" si="2"/>
         <v>3.68E-4</v>
       </c>
     </row>
@@ -18122,15 +18122,15 @@
         <v>100</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.8499999999999995E-4</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.307E-3</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.5200000000000002E-4</v>
       </c>
       <c r="N7" s="2">
@@ -18158,27 +18158,27 @@
         <v>2</v>
       </c>
       <c r="W7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.11E-4</v>
       </c>
       <c r="X7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.728E-3</v>
       </c>
       <c r="Y7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.2766999999999998E-2</v>
       </c>
       <c r="Z7" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.41898099999999999</v>
       </c>
       <c r="AA7" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.9718999999999998</v>
       </c>
       <c r="AB7" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>58.879799999999996</v>
       </c>
       <c r="AD7" s="2">
@@ -18198,11 +18198,11 @@
         <v>100</v>
       </c>
       <c r="AJ7" s="2">
-        <f>AE7*10^-6</f>
+        <f t="shared" si="1"/>
         <v>1.1359999999999999E-3</v>
       </c>
       <c r="AK7" s="2">
-        <f>AF7*10^-6</f>
+        <f t="shared" si="2"/>
         <v>9.4299999999999994E-4</v>
       </c>
     </row>
@@ -18226,15 +18226,15 @@
         <v>500</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5799999999999998E-3</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4088999999999999E-2</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5082E-2</v>
       </c>
       <c r="N8" s="2">
@@ -18262,27 +18262,27 @@
         <v>3</v>
       </c>
       <c r="W8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.5999999999999991E-5</v>
       </c>
       <c r="X8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.8399999999999998E-3</v>
       </c>
       <c r="Y8" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.1545999999999998E-2</v>
       </c>
       <c r="Z8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.373143</v>
       </c>
       <c r="AA8" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.9198999999999997</v>
       </c>
       <c r="AB8" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44.283799999999999</v>
       </c>
       <c r="AD8" s="2">
@@ -18302,11 +18302,11 @@
         <v>500</v>
       </c>
       <c r="AJ8" s="2">
-        <f>AE8*10^-6</f>
+        <f t="shared" si="1"/>
         <v>7.4279999999999997E-3</v>
       </c>
       <c r="AK8" s="2">
-        <f>AF8*10^-6</f>
+        <f t="shared" si="2"/>
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
@@ -18330,15 +18330,15 @@
         <v>1000</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.7090999999999999E-2</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9872E-2</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1438E-2</v>
       </c>
       <c r="N9" s="2">
@@ -18366,27 +18366,27 @@
         <v>4</v>
       </c>
       <c r="W9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.5999999999999991E-5</v>
       </c>
       <c r="X9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.7419999999999998E-3</v>
       </c>
       <c r="Y9" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.3969999999999998E-2</v>
       </c>
       <c r="Z9" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.29074099999999997</v>
       </c>
       <c r="AA9" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.7681</v>
       </c>
       <c r="AB9" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>34.860199999999999</v>
       </c>
       <c r="AD9" s="2">
@@ -18406,11 +18406,11 @@
         <v>1000</v>
       </c>
       <c r="AJ9" s="2">
-        <f>AE9*10^-6</f>
+        <f t="shared" si="1"/>
         <v>2.2443999999999999E-2</v>
       </c>
       <c r="AK9" s="2">
-        <f>AF9*10^-6</f>
+        <f t="shared" si="2"/>
         <v>2.53E-2</v>
       </c>
     </row>
@@ -18434,15 +18434,15 @@
         <v>5000</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.207874</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.32587499999999997</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.533641</v>
       </c>
       <c r="N10" s="2">
@@ -18470,27 +18470,27 @@
         <v>5</v>
       </c>
       <c r="W10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2999999999999996E-5</v>
       </c>
       <c r="X10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.663E-3</v>
       </c>
       <c r="Y10" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.3889999999999998E-2</v>
       </c>
       <c r="Z10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18873199999999998</v>
       </c>
       <c r="AA10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4333999999999998</v>
       </c>
       <c r="AB10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>33.987699999999997</v>
       </c>
       <c r="AD10" s="2">
@@ -18510,11 +18510,11 @@
         <v>5000</v>
       </c>
       <c r="AJ10" s="2">
-        <f>AE10*10^-6</f>
+        <f t="shared" si="1"/>
         <v>0.30603900000000001</v>
       </c>
       <c r="AK10" s="2">
-        <f>AF10*10^-6</f>
+        <f t="shared" si="2"/>
         <v>0.322579</v>
       </c>
     </row>
@@ -18538,15 +18538,15 @@
         <v>10000</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.44919999999999999</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.76199299999999992</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.9546799999999998</v>
       </c>
       <c r="N11" s="2">
@@ -18574,27 +18574,27 @@
         <v>6</v>
       </c>
       <c r="W11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2999999999999996E-5</v>
       </c>
       <c r="X11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2469999999999998E-3</v>
       </c>
       <c r="Y11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.7298999999999998E-2</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.189667</v>
       </c>
       <c r="AA11" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6298999999999997</v>
       </c>
       <c r="AB11" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>33.3643</v>
       </c>
       <c r="AD11" s="2">
@@ -18614,11 +18614,11 @@
         <v>10000</v>
       </c>
       <c r="AJ11" s="2">
-        <f>AE11*10^-6</f>
+        <f t="shared" si="1"/>
         <v>0.92679</v>
       </c>
       <c r="AK11" s="2">
-        <f>AF11*10^-6</f>
+        <f t="shared" si="2"/>
         <v>0.99053999999999998</v>
       </c>
     </row>
@@ -18642,15 +18642,15 @@
         <v>50000</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5564079999999998</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7646929999999994</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153.06752499999999</v>
       </c>
       <c r="N12" s="2">
@@ -18678,27 +18678,27 @@
         <v>7</v>
       </c>
       <c r="W12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2999999999999996E-5</v>
       </c>
       <c r="X12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0999999999999998E-3</v>
       </c>
       <c r="Y12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.5254999999999999E-2</v>
       </c>
       <c r="Z12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.188503</v>
       </c>
       <c r="AA12" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6555</v>
       </c>
       <c r="AB12" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>32.376100000000001</v>
       </c>
       <c r="AD12" s="2">
@@ -18718,11 +18718,11 @@
         <v>50000</v>
       </c>
       <c r="AJ12" s="2">
-        <f>AE12*10^-6</f>
+        <f t="shared" si="1"/>
         <v>3.6861699999999997</v>
       </c>
       <c r="AK12" s="2">
-        <f>AF12*10^-6</f>
+        <f t="shared" si="2"/>
         <v>3.6443699999999999</v>
       </c>
     </row>
@@ -18746,15 +18746,15 @@
         <v>100000</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6542599999999998</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10.49455</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>612.95191</v>
       </c>
       <c r="N13" s="2">
@@ -18782,27 +18782,27 @@
         <v>8</v>
       </c>
       <c r="W13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2999999999999996E-5</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.088E-3</v>
       </c>
       <c r="Y13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2548999999999999E-2</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18775500000000001</v>
       </c>
       <c r="AA13" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6113999999999997</v>
       </c>
       <c r="AB13" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>30.0764</v>
       </c>
       <c r="AD13" s="2">
@@ -18822,11 +18822,11 @@
         <v>100000</v>
       </c>
       <c r="AJ13" s="2">
-        <f>AE13*10^-6</f>
+        <f t="shared" si="1"/>
         <v>8.01539</v>
       </c>
       <c r="AK13" s="2">
-        <f>AF13*10^-6</f>
+        <f t="shared" si="2"/>
         <v>7.2691099999999995</v>
       </c>
     </row>
@@ -18850,15 +18850,15 @@
         <v>500000</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30.291869999999999</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.085839999999997</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16284.815569999999</v>
       </c>
       <c r="N14" s="2">
@@ -18886,27 +18886,27 @@
         <v>9</v>
       </c>
       <c r="W14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2999999999999996E-5</v>
       </c>
       <c r="X14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.3199999999999995E-4</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2591E-2</v>
       </c>
       <c r="Z14" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18412699999999999</v>
       </c>
       <c r="AA14" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.5587999999999997</v>
       </c>
       <c r="AB14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.2393</v>
       </c>
       <c r="AD14" s="2">
@@ -18926,11 +18926,11 @@
         <v>500000</v>
       </c>
       <c r="AJ14" s="2">
-        <f>AE14*10^-6</f>
+        <f t="shared" si="1"/>
         <v>40.117709999999995</v>
       </c>
       <c r="AK14" s="2">
-        <f>AF14*10^-6</f>
+        <f t="shared" si="2"/>
         <v>38.404440000000001</v>
       </c>
     </row>
@@ -18954,11 +18954,11 @@
         <v>1000000</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62.143366</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>123.14403299999999</v>
       </c>
       <c r="K15" s="2">
@@ -18990,27 +18990,27 @@
         <v>10</v>
       </c>
       <c r="W15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.36E-4</v>
       </c>
       <c r="Y15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2600999999999999E-2</v>
       </c>
       <c r="Z15" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18041299999999999</v>
       </c>
       <c r="AA15" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.8130999999999999</v>
       </c>
       <c r="AB15" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.323699999999999</v>
       </c>
       <c r="AD15" s="2">
@@ -19030,11 +19030,11 @@
         <v>1000000</v>
       </c>
       <c r="AJ15" s="2">
-        <f>AE15*10^-6</f>
+        <f t="shared" si="1"/>
         <v>79.238900000000001</v>
       </c>
       <c r="AK15" s="2">
-        <f>AF15*10^-6</f>
+        <f t="shared" si="2"/>
         <v>81.338099999999997</v>
       </c>
     </row>
@@ -19058,11 +19058,11 @@
         <v>5000000</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364.819433</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>538.63530000000003</v>
       </c>
       <c r="N16" s="2">
@@ -19090,27 +19090,27 @@
         <v>11</v>
       </c>
       <c r="W16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.9899999999999997E-4</v>
       </c>
       <c r="Y16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3096E-2</v>
       </c>
       <c r="Z16" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18579399999999999</v>
       </c>
       <c r="AA16" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6303999999999998</v>
       </c>
       <c r="AB16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>30.005099999999999</v>
       </c>
       <c r="AD16" s="2">
@@ -19164,27 +19164,27 @@
         <v>12</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.9199999999999997E-4</v>
       </c>
       <c r="Y17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3352999999999999E-2</v>
       </c>
       <c r="Z17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.166239</v>
       </c>
       <c r="AA17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4127000000000001</v>
       </c>
       <c r="AB17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.206399999999999</v>
       </c>
     </row>
@@ -19214,27 +19214,27 @@
         <v>13</v>
       </c>
       <c r="W18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8299999999999998E-4</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.0267999999999998E-2</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.17206099999999999</v>
       </c>
       <c r="AA18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6056999999999997</v>
       </c>
       <c r="AB18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.171399999999998</v>
       </c>
     </row>
@@ -19264,27 +19264,27 @@
         <v>14</v>
       </c>
       <c r="W19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8299999999999998E-4</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2744E-2</v>
       </c>
       <c r="Z19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18090799999999999</v>
       </c>
       <c r="AA19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3041999999999998</v>
       </c>
       <c r="AB19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.147399999999998</v>
       </c>
     </row>
@@ -19314,27 +19314,27 @@
         <v>15</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9100000000000001E-4</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.4886E-2</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.16432099999999999</v>
       </c>
       <c r="AA20" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3673999999999999</v>
       </c>
       <c r="AB20" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>27.4389</v>
       </c>
     </row>
@@ -19364,27 +19364,27 @@
         <v>16</v>
       </c>
       <c r="W21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.84E-4</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3656E-2</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.16447599999999998</v>
       </c>
       <c r="AA21" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3142999999999998</v>
       </c>
       <c r="AB21" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26.554099999999998</v>
       </c>
     </row>
@@ -19414,27 +19414,27 @@
         <v>17</v>
       </c>
       <c r="W22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8199999999999995E-4</v>
       </c>
       <c r="Y22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1205E-2</v>
       </c>
       <c r="Z22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.17196799999999998</v>
       </c>
       <c r="AA22" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4274</v>
       </c>
       <c r="AB22" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.8171</v>
       </c>
     </row>
@@ -19464,27 +19464,27 @@
         <v>18</v>
       </c>
       <c r="W23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8899999999999996E-4</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1684999999999999E-2</v>
       </c>
       <c r="Z23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.164184</v>
       </c>
       <c r="AA23" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.5994999999999999</v>
       </c>
       <c r="AB23" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26.0426</v>
       </c>
     </row>
@@ -19514,27 +19514,27 @@
         <v>19</v>
       </c>
       <c r="W24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.84E-4</v>
       </c>
       <c r="Y24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0477E-2</v>
       </c>
       <c r="Z24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.20455999999999999</v>
       </c>
       <c r="AA24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3186</v>
       </c>
       <c r="AB24" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.924399999999999</v>
       </c>
     </row>
@@ -19564,27 +19564,27 @@
         <v>20</v>
       </c>
       <c r="W25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8699999999999997E-4</v>
       </c>
       <c r="Y25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0640999999999999E-2</v>
       </c>
       <c r="Z25" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14496000000000001</v>
       </c>
       <c r="AA25" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3828999999999998</v>
       </c>
       <c r="AB25" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.885899999999999</v>
       </c>
     </row>
@@ -19614,27 +19614,27 @@
         <v>21</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.86E-4</v>
       </c>
       <c r="Y26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1712E-2</v>
       </c>
       <c r="Z26" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14486599999999999</v>
       </c>
       <c r="AA26" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4003999999999999</v>
       </c>
       <c r="AB26" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26.558599999999998</v>
       </c>
     </row>
@@ -19664,27 +19664,27 @@
         <v>22</v>
       </c>
       <c r="W27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8499999999999997E-4</v>
       </c>
       <c r="Y27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0914E-2</v>
       </c>
       <c r="Z27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.144423</v>
       </c>
       <c r="AA27" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.3226999999999998</v>
       </c>
       <c r="AB27" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.908799999999999</v>
       </c>
     </row>
@@ -19714,27 +19714,27 @@
         <v>23</v>
       </c>
       <c r="W28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9299999999999995E-4</v>
       </c>
       <c r="Y28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0954999999999999E-2</v>
       </c>
       <c r="Z28" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14427799999999999</v>
       </c>
       <c r="AA28" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.5633999999999997</v>
       </c>
       <c r="AB28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.944699999999997</v>
       </c>
     </row>
@@ -19764,27 +19764,27 @@
         <v>24</v>
       </c>
       <c r="W29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8799999999999999E-4</v>
       </c>
       <c r="Y29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0444999999999999E-2</v>
       </c>
       <c r="Z29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.143539</v>
       </c>
       <c r="AA29" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.2479999999999998</v>
       </c>
       <c r="AB29" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26.045500000000001</v>
       </c>
     </row>
@@ -19814,27 +19814,27 @@
         <v>25</v>
       </c>
       <c r="W30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6199999999999996E-4</v>
       </c>
       <c r="Y30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1564E-2</v>
       </c>
       <c r="Z30" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.148842</v>
       </c>
       <c r="AA30" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.0297999999999998</v>
       </c>
       <c r="AB30" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26.343899999999998</v>
       </c>
     </row>
@@ -19864,27 +19864,27 @@
         <v>26</v>
       </c>
       <c r="W31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6499999999999998E-4</v>
       </c>
       <c r="Y31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3207999999999999E-2</v>
       </c>
       <c r="Z31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14349899999999999</v>
       </c>
       <c r="AA31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.1180999999999996</v>
       </c>
       <c r="AB31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>27.3689</v>
       </c>
     </row>
@@ -19914,27 +19914,27 @@
         <v>27</v>
       </c>
       <c r="W32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.48E-4</v>
       </c>
       <c r="Y32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0995E-2</v>
       </c>
       <c r="Z32" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14469299999999999</v>
       </c>
       <c r="AA32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.1640999999999999</v>
       </c>
       <c r="AB32" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>27.482099999999999</v>
       </c>
     </row>
@@ -19964,27 +19964,27 @@
         <v>28</v>
       </c>
       <c r="W33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.77E-4</v>
       </c>
       <c r="Y33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1112E-2</v>
       </c>
       <c r="Z33" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14396599999999998</v>
       </c>
       <c r="AA33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.944</v>
       </c>
       <c r="AB33" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>27.6111</v>
       </c>
     </row>
@@ -20014,27 +20014,27 @@
         <v>29</v>
       </c>
       <c r="W34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6600000000000001E-4</v>
       </c>
       <c r="Y34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.111E-2</v>
       </c>
       <c r="Z34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.144228</v>
       </c>
       <c r="AA34" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.0648</v>
       </c>
       <c r="AB34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>27.063800000000001</v>
       </c>
     </row>
@@ -20064,27 +20064,27 @@
         <v>30</v>
       </c>
       <c r="W35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="X35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.57E-4</v>
       </c>
       <c r="Y35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0936E-2</v>
       </c>
       <c r="Z35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14373</v>
       </c>
       <c r="AA35" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.2772999999999999</v>
       </c>
       <c r="AB35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25.039199999999997</v>
       </c>
     </row>

</xml_diff>